<commit_message>
update table css and complete import and export bill
</commit_message>
<xml_diff>
--- a/baocao/phieu_nhap_xuat.xlsx
+++ b/baocao/phieu_nhap_xuat.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t>QC PHÒNG KHÔNG - KHÔNG QUÂN</t>
   </si>
@@ -304,34 +304,28 @@
     <t>2024-12-04</t>
   </si>
   <si>
-    <t>e927</t>
-  </si>
-  <si>
-    <t>Xuất báo nợ</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>2024-12-13</t>
-  </si>
-  <si>
-    <t>2024-12-12</t>
-  </si>
-  <si>
-    <t>A80</t>
-  </si>
-  <si>
-    <t>Xăng A80</t>
+    <t>e923</t>
+  </si>
+  <si>
+    <t>Tác chiến cho bay</t>
+  </si>
+  <si>
+    <t>2024-12-21</t>
+  </si>
+  <si>
+    <t>2024-12-20</t>
+  </si>
+  <si>
+    <t>JETA-01</t>
+  </si>
+  <si>
+    <t>Dầu JETA-01</t>
   </si>
   <si>
     <t>0.0</t>
-  </si>
-  <si>
-    <t>E5-RON92</t>
-  </si>
-  <si>
-    <t>XANG E5 RON92</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1779,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P27"/>
+  <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1855,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="9" t="n">
-        <v>2154.0</v>
+        <v>2381.0</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
@@ -1872,7 +1866,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="68" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -1887,7 +1881,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L5" s="70"/>
     </row>
@@ -1897,7 +1891,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="68" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1916,7 +1910,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="71" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -1935,7 +1929,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="71" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -2043,7 +2037,7 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="29" t="n">
-        <v>11.0</v>
+        <v>2026.0</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>68</v>
@@ -2055,50 +2049,30 @@
         <v>0.0</v>
       </c>
       <c r="J13" s="30" t="n">
-        <v>13.0</v>
+        <v>2026.0</v>
       </c>
       <c r="K13" s="30" t="n">
         <v>142857.0</v>
       </c>
       <c r="L13" s="30" t="n">
-        <v>1857141.0</v>
+        <v>2.89428282E8</v>
       </c>
       <c r="P13" s="31"/>
     </row>
     <row r="14" ht="20.85" customHeight="true">
-      <c r="B14" s="32" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="33"/>
-      <c r="F14" s="34" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J14" s="35" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="K14" s="35" t="n">
-        <v>3548.0</v>
-      </c>
-      <c r="L14" s="35" t="n">
-        <v>21288.0</v>
-      </c>
-    </row>
-    <row r="15" ht="20.85" customHeight="true">
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="2:16" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
@@ -2111,125 +2085,125 @@
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="2:16" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-    </row>
-    <row r="17" spans="2:16" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37" t="s">
+    <row r="16" spans="2:16" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="73" t="n">
-        <f>SUM(J13:J16)</f>
-        <v>19.0</v>
-      </c>
-      <c r="K17" s="73"/>
-      <c r="L17" s="39" t="n">
-        <f>SUM(L13:L16)</f>
-        <v>1878429.0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="73" t="n">
+        <f>SUM(J13:J15)</f>
+        <v>2026.0</v>
+      </c>
+      <c r="K16" s="73"/>
+      <c r="L16" s="39" t="n">
+        <f>SUM(L13:L15)</f>
+        <v>2.89428282E8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="46"/>
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="2:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="46"/>
-      <c r="P18" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="2:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="51"/>
-    </row>
-    <row r="20" spans="2:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="54"/>
-    </row>
-    <row r="21" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="90"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="54"/>
+    </row>
+    <row r="20" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="90"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="80"/>
+      <c r="K21" s="90" t="s">
+        <v>43</v>
+      </c>
       <c r="L21" s="90"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="79" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="80"/>
-      <c r="K22" s="90" t="s">
-        <v>43</v>
-      </c>
-      <c r="L22" s="90"/>
+    <row r="22" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="59"/>
     </row>
     <row r="23" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="56"/>
@@ -2245,67 +2219,54 @@
       <c r="L23" s="59"/>
     </row>
     <row r="24" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="59"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="64"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="64"/>
-    </row>
-    <row r="26" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="74" t="s">
+      <c r="B25" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76" t="s">
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76" t="s">
+      <c r="H25" s="76"/>
+      <c r="I25" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="76"/>
-      <c r="K26" s="89" t="s">
+      <c r="J25" s="76"/>
+      <c r="K25" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="L26" s="89"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
+      <c r="L25" s="89"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="33">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="K2:L2"/>
@@ -2317,17 +2278,17 @@
     <mergeCell ref="F11:J11"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
     <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lỗi" error="Vui lòng chọn dữ liệu trong danh sách. (Add-in A-Tools Tác giả: Nguyễn Duy Tuân - http://bluesofts.net)" sqref="H4">

</xml_diff>